<commit_message>
add plotting functions with bug fixes
</commit_message>
<xml_diff>
--- a/results/performance_scores.xlsx
+++ b/results/performance_scores.xlsx
@@ -528,10 +528,10 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0.3021624295738912</v>
+        <v>0.2502814507848615</v>
       </c>
       <c r="E2" t="n">
-        <v>0.6978375704261088</v>
+        <v>0.7497185492151386</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add part one of the workshop example
</commit_message>
<xml_diff>
--- a/results/performance_scores.xlsx
+++ b/results/performance_scores.xlsx
@@ -528,10 +528,10 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0.2502814507848615</v>
+        <v>0.143931018344888</v>
       </c>
       <c r="E2" t="n">
-        <v>0.7497185492151386</v>
+        <v>0.8560689816551121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finish the complete workshop example
</commit_message>
<xml_diff>
--- a/results/performance_scores.xlsx
+++ b/results/performance_scores.xlsx
@@ -528,10 +528,10 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0.143931018344888</v>
+        <v>0.3520219424078004</v>
       </c>
       <c r="E2" t="n">
-        <v>0.8560689816551121</v>
+        <v>0.6479780575921996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add interactive jupyter notebook
</commit_message>
<xml_diff>
--- a/results/performance_scores.xlsx
+++ b/results/performance_scores.xlsx
@@ -528,10 +528,10 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0.3520219424078004</v>
+        <v>0.2845178558249991</v>
       </c>
       <c r="E2" t="n">
-        <v>0.6479780575921996</v>
+        <v>0.715482144175001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update workshop interactive module
</commit_message>
<xml_diff>
--- a/results/performance_scores.xlsx
+++ b/results/performance_scores.xlsx
@@ -528,10 +528,10 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0.2845178558249991</v>
+        <v>0.4448392219969687</v>
       </c>
       <c r="E2" t="n">
-        <v>0.715482144175001</v>
+        <v>0.5551607780030313</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add environment.yml for binder
</commit_message>
<xml_diff>
--- a/results/performance_scores.xlsx
+++ b/results/performance_scores.xlsx
@@ -528,10 +528,10 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0.4448392219969687</v>
+        <v>0.2556232321110647</v>
       </c>
       <c r="E2" t="n">
-        <v>0.5551607780030313</v>
+        <v>0.7443767678889354</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add interactive system/TEA/LCA/MCDA modules
</commit_message>
<xml_diff>
--- a/results/performance_scores.xlsx
+++ b/results/performance_scores.xlsx
@@ -458,7 +458,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1:1</t>
+          <t>1:0</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -468,7 +468,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>sysB</t>
+          <t>sysA</t>
         </is>
       </c>
     </row>
@@ -519,7 +519,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1:1</t>
+          <t>1:0</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -528,10 +528,10 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0.2556232321110647</v>
+        <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>0.7443767678889354</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -581,7 +581,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1:1</t>
+          <t>1:0</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -590,10 +590,10 @@
         </is>
       </c>
       <c r="D2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" t="n">
         <v>2</v>
-      </c>
-      <c r="E2" t="n">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
try to revive binder through pushing
</commit_message>
<xml_diff>
--- a/results/performance_scores.xlsx
+++ b/results/performance_scores.xlsx
@@ -458,7 +458,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>0.5:0.5</t>
+          <t>0.82:0.18</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -468,7 +468,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>sysB</t>
+          <t>sysA</t>
         </is>
       </c>
     </row>
@@ -519,7 +519,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>0.5:0.5</t>
+          <t>0.82:0.18</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -528,10 +528,10 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0.2844662572099641</v>
+        <v>0.6447682538072267</v>
       </c>
       <c r="E2" t="n">
-        <v>0.7155337427900359</v>
+        <v>0.3552317461927733</v>
       </c>
     </row>
   </sheetData>
@@ -581,7 +581,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>0.5:0.5</t>
+          <t>0.82:0.18</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -590,10 +590,10 @@
         </is>
       </c>
       <c r="D2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" t="n">
         <v>2</v>
-      </c>
-      <c r="E2" t="n">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add metric unit to interactive UA/SA module, update README with new binder instruction
</commit_message>
<xml_diff>
--- a/results/performance_scores.xlsx
+++ b/results/performance_scores.xlsx
@@ -27,7 +27,7 @@
     <t>Winner</t>
   </si>
   <si>
-    <t>0.5:0.5</t>
+    <t>1:0</t>
   </si>
   <si>
     <t>Econ, Env</t>
@@ -463,10 +463,10 @@
         <v>4</v>
       </c>
       <c r="D2">
-        <v>0.2844662572099641</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>0.7155337427900359</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>